<commit_message>
FEB batch dataprovider and suit execution
</commit_message>
<xml_diff>
--- a/src/test/resources/data/hr.xlsx
+++ b/src/test/resources/data/hr.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7050"/>
+    <workbookView windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,21 +28,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>somedata</t>
   </si>
   <si>
     <t>user1</t>
@@ -51,16 +42,22 @@
     <t>pass@123</t>
   </si>
   <si>
-    <t>user1@gmail.com</t>
-  </si>
-  <si>
     <t>user2</t>
   </si>
   <si>
     <t>pass@124</t>
   </si>
   <si>
-    <t>user2@gmail.com</t>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>pass@125</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>pass@126</t>
   </si>
 </sst>
 </file>
@@ -996,68 +993,66 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
+    <col min="2" max="2" width="10.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="11.7142857142857"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>7767007446</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3">
-        <v>7767007447</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="pass@123"/>
-    <hyperlink ref="D2" r:id="rId2" display="user1@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId1" display="pass@126"/>
     <hyperlink ref="B3" r:id="rId1" display="pass@124"/>
-    <hyperlink ref="D3" r:id="rId2" display="user2@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="pass@125"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1067,14 +1062,61 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="pass@123"/>
+    <hyperlink ref="B5" r:id="rId1" display="pass@126"/>
+    <hyperlink ref="B3" r:id="rId1" display="pass@124"/>
+    <hyperlink ref="B4" r:id="rId1" display="pass@125"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>